<commit_message>
added feedback form link
</commit_message>
<xml_diff>
--- a/public/assets/img/pics/Copie de catalogue online 11_09_2019.xlsx
+++ b/public/assets/img/pics/Copie de catalogue online 11_09_2019.xlsx
@@ -75,7 +75,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4332" uniqueCount="1733">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4333" uniqueCount="1734">
   <si>
     <t>article_code</t>
   </si>
@@ -6496,6 +6496,9 @@
   </si>
   <si>
     <t>CSHETENM72- pict 1 and CSHETENM72- pict 2</t>
+  </si>
+  <si>
+    <t>Inner tubes</t>
   </si>
 </sst>
 </file>
@@ -7244,7 +7247,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -7252,12 +7255,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:Q481"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O129" sqref="O129"/>
+      <pane ySplit="1" topLeftCell="A468" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B475" sqref="B475"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7330,7 +7332,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="28" t="s">
         <v>1309</v>
       </c>
@@ -7372,7 +7374,7 @@
       </c>
       <c r="Q2" s="16"/>
     </row>
-    <row r="3" spans="1:17" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
         <v>1311</v>
       </c>
@@ -7414,7 +7416,7 @@
       </c>
       <c r="Q3" s="65"/>
     </row>
-    <row r="4" spans="1:17" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
         <v>1313</v>
       </c>
@@ -7456,7 +7458,7 @@
       </c>
       <c r="Q4" s="67"/>
     </row>
-    <row r="5" spans="1:17" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="16" t="s">
         <v>1315</v>
       </c>
@@ -7498,7 +7500,7 @@
       </c>
       <c r="Q5" s="67"/>
     </row>
-    <row r="6" spans="1:17" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
         <v>1317</v>
       </c>
@@ -7540,7 +7542,7 @@
       </c>
       <c r="Q6" s="65"/>
     </row>
-    <row r="7" spans="1:17" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="16" t="s">
         <v>1319</v>
       </c>
@@ -7582,7 +7584,7 @@
       </c>
       <c r="Q7" s="65"/>
     </row>
-    <row r="8" spans="1:17" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="16" t="s">
         <v>1321</v>
       </c>
@@ -7624,7 +7626,7 @@
       </c>
       <c r="Q8" s="67"/>
     </row>
-    <row r="9" spans="1:17" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="16" t="s">
         <v>1323</v>
       </c>
@@ -7666,7 +7668,7 @@
       </c>
       <c r="Q9" s="67"/>
     </row>
-    <row r="10" spans="1:17" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="16" t="s">
         <v>1325</v>
       </c>
@@ -7708,7 +7710,7 @@
       </c>
       <c r="Q10" s="67"/>
     </row>
-    <row r="11" spans="1:17" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="16" t="s">
         <v>162</v>
       </c>
@@ -7750,7 +7752,7 @@
       </c>
       <c r="Q11" s="8"/>
     </row>
-    <row r="12" spans="1:17" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="16" t="s">
         <v>1328</v>
       </c>
@@ -7792,7 +7794,7 @@
       </c>
       <c r="Q12" s="38"/>
     </row>
-    <row r="13" spans="1:17" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="16" t="s">
         <v>1330</v>
       </c>
@@ -7834,7 +7836,7 @@
       </c>
       <c r="Q13" s="38"/>
     </row>
-    <row r="14" spans="1:17" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
         <v>1332</v>
       </c>
@@ -7876,7 +7878,7 @@
       </c>
       <c r="Q14" s="38"/>
     </row>
-    <row r="15" spans="1:17" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="16" t="s">
         <v>1334</v>
       </c>
@@ -7918,7 +7920,7 @@
       </c>
       <c r="Q15" s="8"/>
     </row>
-    <row r="16" spans="1:17" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="16" t="s">
         <v>1336</v>
       </c>
@@ -7960,7 +7962,7 @@
       </c>
       <c r="Q16" s="3"/>
     </row>
-    <row r="17" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
         <v>1338</v>
       </c>
@@ -7995,7 +7997,7 @@
         <v>810</v>
       </c>
     </row>
-    <row r="18" spans="1:17" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="16" t="s">
         <v>1340</v>
       </c>
@@ -8037,7 +8039,7 @@
       </c>
       <c r="Q18" s="69"/>
     </row>
-    <row r="19" spans="1:17" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="16" t="s">
         <v>1342</v>
       </c>
@@ -8079,7 +8081,7 @@
       </c>
       <c r="Q19" s="8"/>
     </row>
-    <row r="20" spans="1:17" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="16" t="s">
         <v>1344</v>
       </c>
@@ -8121,7 +8123,7 @@
       </c>
       <c r="Q20" s="8"/>
     </row>
-    <row r="21" spans="1:17" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="16" t="s">
         <v>1346</v>
       </c>
@@ -8163,7 +8165,7 @@
       </c>
       <c r="Q21" s="8"/>
     </row>
-    <row r="22" spans="1:17" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="16" t="s">
         <v>1348</v>
       </c>
@@ -8205,7 +8207,7 @@
       </c>
       <c r="Q22" s="8"/>
     </row>
-    <row r="23" spans="1:17" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="16" t="s">
         <v>1350</v>
       </c>
@@ -8247,7 +8249,7 @@
       </c>
       <c r="Q23" s="8"/>
     </row>
-    <row r="24" spans="1:17" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="16" t="s">
         <v>1352</v>
       </c>
@@ -8289,7 +8291,7 @@
       </c>
       <c r="Q24" s="8"/>
     </row>
-    <row r="25" spans="1:17" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="16" t="s">
         <v>1354</v>
       </c>
@@ -8331,7 +8333,7 @@
       </c>
       <c r="Q25" s="38"/>
     </row>
-    <row r="26" spans="1:17" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="16" t="s">
         <v>1356</v>
       </c>
@@ -8373,7 +8375,7 @@
       </c>
       <c r="Q26" s="8"/>
     </row>
-    <row r="27" spans="1:17" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="16" t="s">
         <v>1358</v>
       </c>
@@ -8415,7 +8417,7 @@
       </c>
       <c r="Q27" s="8"/>
     </row>
-    <row r="28" spans="1:17" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="16" t="s">
         <v>1360</v>
       </c>
@@ -8457,7 +8459,7 @@
       </c>
       <c r="Q28" s="8"/>
     </row>
-    <row r="29" spans="1:17" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="16" t="s">
         <v>1362</v>
       </c>
@@ -8499,7 +8501,7 @@
       </c>
       <c r="Q29" s="8"/>
     </row>
-    <row r="30" spans="1:17" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="16" t="s">
         <v>1364</v>
       </c>
@@ -8541,7 +8543,7 @@
       </c>
       <c r="Q30" s="8"/>
     </row>
-    <row r="31" spans="1:17" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="16" t="s">
         <v>1366</v>
       </c>
@@ -8583,7 +8585,7 @@
       </c>
       <c r="Q31" s="3"/>
     </row>
-    <row r="32" spans="1:17" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="16" t="s">
         <v>1368</v>
       </c>
@@ -8625,7 +8627,7 @@
       </c>
       <c r="Q32" s="8"/>
     </row>
-    <row r="33" spans="1:17" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="16" t="s">
         <v>1370</v>
       </c>
@@ -8667,7 +8669,7 @@
       </c>
       <c r="Q33" s="38"/>
     </row>
-    <row r="34" spans="1:17" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="16" t="s">
         <v>931</v>
       </c>
@@ -8709,7 +8711,7 @@
       </c>
       <c r="Q34" s="8"/>
     </row>
-    <row r="35" spans="1:17" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="16" t="s">
         <v>1373</v>
       </c>
@@ -8751,7 +8753,7 @@
       </c>
       <c r="Q35" s="8"/>
     </row>
-    <row r="36" spans="1:17" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="16" t="s">
         <v>1375</v>
       </c>
@@ -8793,7 +8795,7 @@
       </c>
       <c r="Q36" s="8"/>
     </row>
-    <row r="37" spans="1:17" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="16" t="s">
         <v>1377</v>
       </c>
@@ -8835,7 +8837,7 @@
       </c>
       <c r="Q37" s="8"/>
     </row>
-    <row r="38" spans="1:17" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="16" t="s">
         <v>1379</v>
       </c>
@@ -8877,7 +8879,7 @@
       </c>
       <c r="Q38" s="38"/>
     </row>
-    <row r="39" spans="1:17" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="16" t="s">
         <v>1381</v>
       </c>
@@ -8919,7 +8921,7 @@
       </c>
       <c r="Q39" s="8"/>
     </row>
-    <row r="40" spans="1:17" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="16" t="s">
         <v>1383</v>
       </c>
@@ -8961,7 +8963,7 @@
       </c>
       <c r="Q40" s="8"/>
     </row>
-    <row r="41" spans="1:17" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="16" t="s">
         <v>1385</v>
       </c>
@@ -9003,7 +9005,7 @@
       </c>
       <c r="Q41" s="8"/>
     </row>
-    <row r="42" spans="1:17" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="16" t="s">
         <v>1387</v>
       </c>
@@ -9045,7 +9047,7 @@
       </c>
       <c r="Q42" s="8"/>
     </row>
-    <row r="43" spans="1:17" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="16" t="s">
         <v>1389</v>
       </c>
@@ -9087,7 +9089,7 @@
       </c>
       <c r="Q43" s="8"/>
     </row>
-    <row r="44" spans="1:17" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="16" t="s">
         <v>1391</v>
       </c>
@@ -9129,7 +9131,7 @@
       </c>
       <c r="Q44" s="8"/>
     </row>
-    <row r="45" spans="1:17" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="16" t="s">
         <v>913</v>
       </c>
@@ -9171,7 +9173,7 @@
       </c>
       <c r="Q45" s="38"/>
     </row>
-    <row r="46" spans="1:17" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="16" t="s">
         <v>914</v>
       </c>
@@ -9213,7 +9215,7 @@
       </c>
       <c r="Q46" s="8"/>
     </row>
-    <row r="47" spans="1:17" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="16" t="s">
         <v>1395</v>
       </c>
@@ -9255,7 +9257,7 @@
       </c>
       <c r="Q47" s="3"/>
     </row>
-    <row r="48" spans="1:17" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="16" t="s">
         <v>1397</v>
       </c>
@@ -9297,7 +9299,7 @@
       </c>
       <c r="Q48" s="3"/>
     </row>
-    <row r="49" spans="1:17" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="16" t="s">
         <v>1399</v>
       </c>
@@ -9339,7 +9341,7 @@
       </c>
       <c r="Q49" s="8"/>
     </row>
-    <row r="50" spans="1:17" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="16" t="s">
         <v>1401</v>
       </c>
@@ -9381,7 +9383,7 @@
       </c>
       <c r="Q50" s="8"/>
     </row>
-    <row r="51" spans="1:17" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="16" t="s">
         <v>167</v>
       </c>
@@ -9423,7 +9425,7 @@
       </c>
       <c r="Q51" s="8"/>
     </row>
-    <row r="52" spans="1:17" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="16" t="s">
         <v>1404</v>
       </c>
@@ -9465,7 +9467,7 @@
       </c>
       <c r="Q52" s="8"/>
     </row>
-    <row r="53" spans="1:17" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="16" t="s">
         <v>926</v>
       </c>
@@ -9507,7 +9509,7 @@
       </c>
       <c r="Q53" s="8"/>
     </row>
-    <row r="54" spans="1:17" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="16" t="s">
         <v>927</v>
       </c>
@@ -9549,7 +9551,7 @@
       </c>
       <c r="Q54" s="8"/>
     </row>
-    <row r="55" spans="1:17" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="16" t="s">
         <v>1408</v>
       </c>
@@ -9591,7 +9593,7 @@
       </c>
       <c r="Q55" s="8"/>
     </row>
-    <row r="56" spans="1:17" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="16" t="s">
         <v>1410</v>
       </c>
@@ -9633,7 +9635,7 @@
       </c>
       <c r="Q56" s="8"/>
     </row>
-    <row r="57" spans="1:17" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="16" t="s">
         <v>1412</v>
       </c>
@@ -9675,7 +9677,7 @@
       </c>
       <c r="Q57" s="8"/>
     </row>
-    <row r="58" spans="1:17" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="16" t="s">
         <v>1414</v>
       </c>
@@ -9717,7 +9719,7 @@
       </c>
       <c r="Q58" s="8"/>
     </row>
-    <row r="59" spans="1:17" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="16" t="s">
         <v>1416</v>
       </c>
@@ -9759,7 +9761,7 @@
       </c>
       <c r="Q59" s="8"/>
     </row>
-    <row r="60" spans="1:17" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="16" t="s">
         <v>1418</v>
       </c>
@@ -9801,7 +9803,7 @@
       </c>
       <c r="Q60" s="8"/>
     </row>
-    <row r="61" spans="1:17" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="16" t="s">
         <v>1420</v>
       </c>
@@ -9843,7 +9845,7 @@
       </c>
       <c r="Q61" s="8"/>
     </row>
-    <row r="62" spans="1:17" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="16" t="s">
         <v>160</v>
       </c>
@@ -9893,7 +9895,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="63" spans="1:17" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="16" t="s">
         <v>161</v>
       </c>
@@ -9943,7 +9945,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="64" spans="1:17" ht="270" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:17" ht="270" x14ac:dyDescent="0.25">
       <c r="A64" s="8" t="s">
         <v>873</v>
       </c>
@@ -9987,7 +9989,7 @@
         <v>875</v>
       </c>
     </row>
-    <row r="65" spans="1:17" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="6" t="s">
         <v>881</v>
       </c>
@@ -10032,7 +10034,7 @@
       </c>
       <c r="Q65" s="28"/>
     </row>
-    <row r="66" spans="1:17" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="14" t="s">
         <v>882</v>
       </c>
@@ -10079,7 +10081,7 @@
         <v>886</v>
       </c>
     </row>
-    <row r="67" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A67" s="19" t="s">
         <v>888</v>
       </c>
@@ -10108,7 +10110,7 @@
         <v>888</v>
       </c>
     </row>
-    <row r="68" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A68" s="19" t="s">
         <v>890</v>
       </c>
@@ -10137,7 +10139,7 @@
         <v>888</v>
       </c>
     </row>
-    <row r="69" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A69" s="19" t="s">
         <v>892</v>
       </c>
@@ -10166,7 +10168,7 @@
         <v>888</v>
       </c>
     </row>
-    <row r="70" spans="1:17" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A70" s="6" t="s">
         <v>895</v>
       </c>
@@ -10207,7 +10209,7 @@
         <v>897</v>
       </c>
     </row>
-    <row r="71" spans="1:17" ht="409.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:17" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A71" s="32" t="s">
         <v>1647</v>
       </c>
@@ -10248,7 +10250,7 @@
         <v>1647</v>
       </c>
     </row>
-    <row r="72" spans="1:17" ht="285" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:17" ht="285" x14ac:dyDescent="0.25">
       <c r="A72" s="19" t="s">
         <v>903</v>
       </c>
@@ -10280,7 +10282,7 @@
         <v>903</v>
       </c>
     </row>
-    <row r="73" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A73" s="60" t="s">
         <v>906</v>
       </c>
@@ -10315,7 +10317,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="74" spans="1:17" s="9" customFormat="1" ht="180" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:17" s="9" customFormat="1" ht="180" x14ac:dyDescent="0.25">
       <c r="A74" s="6" t="s">
         <v>908</v>
       </c>
@@ -10363,7 +10365,7 @@
       </c>
       <c r="Q74" s="28"/>
     </row>
-    <row r="75" spans="1:17" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A75" s="16" t="s">
         <v>911</v>
       </c>
@@ -10408,7 +10410,7 @@
       </c>
       <c r="Q75" s="8"/>
     </row>
-    <row r="76" spans="1:17" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A76" s="16" t="s">
         <v>922</v>
       </c>
@@ -10453,7 +10455,7 @@
       </c>
       <c r="Q76" s="8"/>
     </row>
-    <row r="77" spans="1:17" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A77" s="9" t="s">
         <v>162</v>
       </c>
@@ -10503,7 +10505,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="78" spans="1:17" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A78" s="9" t="s">
         <v>925</v>
       </c>
@@ -10548,7 +10550,7 @@
       </c>
       <c r="Q78" s="8"/>
     </row>
-    <row r="79" spans="1:17" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A79" s="9" t="s">
         <v>923</v>
       </c>
@@ -10593,7 +10595,7 @@
       </c>
       <c r="Q79" s="8"/>
     </row>
-    <row r="80" spans="1:17" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A80" s="9" t="s">
         <v>163</v>
       </c>
@@ -10643,7 +10645,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="81" spans="1:17" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:17" ht="60" x14ac:dyDescent="0.25">
       <c r="A81" s="8" t="s">
         <v>29</v>
       </c>
@@ -10678,7 +10680,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="82" spans="1:17" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A82" s="8" t="s">
         <v>33</v>
       </c>
@@ -10716,7 +10718,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="83" spans="1:17" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:17" ht="60" x14ac:dyDescent="0.25">
       <c r="A83" s="8" t="s">
         <v>35</v>
       </c>
@@ -10754,7 +10756,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="84" spans="1:17" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:17" ht="60" x14ac:dyDescent="0.25">
       <c r="A84" s="8" t="s">
         <v>36</v>
       </c>
@@ -10792,7 +10794,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="85" spans="1:17" s="9" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:17" s="9" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A85" s="9" t="s">
         <v>38</v>
       </c>
@@ -10837,7 +10839,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="86" spans="1:17" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:17" ht="60" x14ac:dyDescent="0.25">
       <c r="A86" s="8" t="s">
         <v>40</v>
       </c>
@@ -10875,7 +10877,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="87" spans="1:17" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:17" ht="60" x14ac:dyDescent="0.25">
       <c r="A87" s="8" t="s">
         <v>41</v>
       </c>
@@ -10913,7 +10915,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="88" spans="1:17" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A88" s="8" t="s">
         <v>44</v>
       </c>
@@ -10951,7 +10953,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="89" spans="1:17" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:17" ht="60" x14ac:dyDescent="0.25">
       <c r="A89" s="8" t="s">
         <v>45</v>
       </c>
@@ -10989,7 +10991,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="90" spans="1:17" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:17" ht="60" x14ac:dyDescent="0.25">
       <c r="A90" s="8" t="s">
         <v>46</v>
       </c>
@@ -11027,7 +11029,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="91" spans="1:17" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:17" ht="60" x14ac:dyDescent="0.25">
       <c r="A91" s="8" t="s">
         <v>48</v>
       </c>
@@ -11065,7 +11067,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="92" spans="1:17" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A92" s="8" t="s">
         <v>49</v>
       </c>
@@ -11103,7 +11105,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="93" spans="1:17" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:17" ht="60" x14ac:dyDescent="0.25">
       <c r="A93" s="8" t="s">
         <v>50</v>
       </c>
@@ -11141,7 +11143,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="94" spans="1:17" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A94" s="8" t="s">
         <v>55</v>
       </c>
@@ -11179,7 +11181,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="95" spans="1:17" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A95" s="8" t="s">
         <v>56</v>
       </c>
@@ -11217,7 +11219,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="96" spans="1:17" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:17" ht="60" x14ac:dyDescent="0.25">
       <c r="A96" s="8" t="s">
         <v>58</v>
       </c>
@@ -11255,7 +11257,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="97" spans="1:17" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A97" s="8" t="s">
         <v>62</v>
       </c>
@@ -11293,7 +11295,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="98" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A98" s="8" t="s">
         <v>63</v>
       </c>
@@ -11331,7 +11333,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="99" spans="1:17" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:17" ht="60" x14ac:dyDescent="0.25">
       <c r="A99" s="8" t="s">
         <v>65</v>
       </c>
@@ -11369,7 +11371,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="100" spans="1:17" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:17" ht="60" x14ac:dyDescent="0.25">
       <c r="A100" s="8" t="s">
         <v>66</v>
       </c>
@@ -11407,7 +11409,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="101" spans="1:17" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A101" s="8" t="s">
         <v>67</v>
       </c>
@@ -11445,7 +11447,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="102" spans="1:17" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A102" s="8" t="s">
         <v>68</v>
       </c>
@@ -11483,7 +11485,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="103" spans="1:17" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:17" ht="60" x14ac:dyDescent="0.25">
       <c r="A103" s="8" t="s">
         <v>70</v>
       </c>
@@ -11521,7 +11523,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="104" spans="1:17" s="9" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:17" s="9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A104" s="9" t="s">
         <v>73</v>
       </c>
@@ -11563,7 +11565,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="105" spans="1:17" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A105" s="8" t="s">
         <v>113</v>
       </c>
@@ -11601,7 +11603,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="106" spans="1:17" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A106" s="9" t="s">
         <v>129</v>
       </c>
@@ -11651,7 +11653,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="107" spans="1:17" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A107" s="9" t="s">
         <v>130</v>
       </c>
@@ -11701,7 +11703,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="108" spans="1:17" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A108" s="8" t="s">
         <v>131</v>
       </c>
@@ -11739,7 +11741,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="109" spans="1:17" s="9" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:17" s="9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A109" s="9" t="s">
         <v>137</v>
       </c>
@@ -11789,7 +11791,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="110" spans="1:17" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A110" s="8" t="s">
         <v>140</v>
       </c>
@@ -11827,7 +11829,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="111" spans="1:17" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A111" s="8" t="s">
         <v>141</v>
       </c>
@@ -11865,7 +11867,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="112" spans="1:17" s="9" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:17" s="9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A112" s="9" t="s">
         <v>151</v>
       </c>
@@ -11915,7 +11917,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="113" spans="1:17" s="9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:17" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A113" s="9" t="s">
         <v>152</v>
       </c>
@@ -11965,7 +11967,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="114" spans="1:17" s="9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:17" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A114" s="9" t="s">
         <v>153</v>
       </c>
@@ -12015,7 +12017,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="115" spans="1:17" s="9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:17" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A115" s="9" t="s">
         <v>154</v>
       </c>
@@ -12065,7 +12067,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="116" spans="1:17" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A116" s="8" t="s">
         <v>155</v>
       </c>
@@ -12109,7 +12111,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="117" spans="1:17" s="9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:17" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A117" s="9" t="s">
         <v>156</v>
       </c>
@@ -12159,7 +12161,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="118" spans="1:17" s="9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:17" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A118" s="9" t="s">
         <v>157</v>
       </c>
@@ -12209,7 +12211,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="119" spans="1:17" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A119" s="8" t="s">
         <v>158</v>
       </c>
@@ -12247,7 +12249,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="120" spans="1:17" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A120" s="8" t="s">
         <v>159</v>
       </c>
@@ -12285,7 +12287,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="121" spans="1:17" ht="375" hidden="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:17" ht="375" x14ac:dyDescent="0.25">
       <c r="A121" s="8" t="s">
         <v>125</v>
       </c>
@@ -12323,7 +12325,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="122" spans="1:17" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A122" s="16" t="s">
         <v>145</v>
       </c>
@@ -12373,7 +12375,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="123" spans="1:17" s="9" customFormat="1" ht="90" hidden="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:17" s="9" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A123" s="17" t="s">
         <v>770</v>
       </c>
@@ -12417,7 +12419,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="124" spans="1:17" ht="90" hidden="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:17" ht="90" x14ac:dyDescent="0.25">
       <c r="A124" s="24" t="s">
         <v>772</v>
       </c>
@@ -12455,7 +12457,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="125" spans="1:17" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A125" s="17" t="s">
         <v>778</v>
       </c>
@@ -12494,7 +12496,7 @@
       </c>
       <c r="Q125" s="28"/>
     </row>
-    <row r="126" spans="1:17" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A126" s="17" t="s">
         <v>780</v>
       </c>
@@ -12568,7 +12570,7 @@
         <v>788</v>
       </c>
     </row>
-    <row r="128" spans="1:17" s="9" customFormat="1" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:17" s="9" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A128" s="6" t="s">
         <v>789</v>
       </c>
@@ -12653,7 +12655,7 @@
         <v>788</v>
       </c>
     </row>
-    <row r="130" spans="1:17" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A130" s="18" t="s">
         <v>800</v>
       </c>
@@ -12691,7 +12693,7 @@
         <v>804</v>
       </c>
     </row>
-    <row r="131" spans="1:17" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A131" s="6" t="s">
         <v>805</v>
       </c>
@@ -12738,7 +12740,7 @@
         <v>809</v>
       </c>
     </row>
-    <row r="132" spans="1:17" s="9" customFormat="1" ht="409.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:17" s="9" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A132" s="6" t="s">
         <v>812</v>
       </c>
@@ -12788,7 +12790,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="133" spans="1:17" s="9" customFormat="1" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:17" s="9" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A133" s="6" t="s">
         <v>817</v>
       </c>
@@ -12838,7 +12840,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="134" spans="1:17" s="9" customFormat="1" ht="409.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:17" s="9" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A134" s="14" t="s">
         <v>825</v>
       </c>
@@ -12888,7 +12890,7 @@
         <v>829</v>
       </c>
     </row>
-    <row r="135" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A135" s="19" t="s">
         <v>831</v>
       </c>
@@ -12920,7 +12922,7 @@
         <v>831</v>
       </c>
     </row>
-    <row r="136" spans="1:17" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A136" s="19" t="s">
         <v>835</v>
       </c>
@@ -12955,7 +12957,7 @@
         <v>859</v>
       </c>
     </row>
-    <row r="137" spans="1:17" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A137" s="19" t="s">
         <v>837</v>
       </c>
@@ -12990,7 +12992,7 @@
         <v>859</v>
       </c>
     </row>
-    <row r="138" spans="1:17" s="9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:17" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A138" s="6" t="s">
         <v>839</v>
       </c>
@@ -13030,7 +13032,7 @@
       </c>
       <c r="Q138" s="39"/>
     </row>
-    <row r="139" spans="1:17" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A139" s="19" t="s">
         <v>841</v>
       </c>
@@ -13062,7 +13064,7 @@
         <v>859</v>
       </c>
     </row>
-    <row r="140" spans="1:17" s="9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:17" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A140" s="6" t="s">
         <v>843</v>
       </c>
@@ -13104,7 +13106,7 @@
       </c>
       <c r="Q140" s="28"/>
     </row>
-    <row r="141" spans="1:17" s="9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:17" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A141" s="6" t="s">
         <v>845</v>
       </c>
@@ -13146,7 +13148,7 @@
       </c>
       <c r="Q141" s="3"/>
     </row>
-    <row r="142" spans="1:17" s="9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:17" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A142" s="6" t="s">
         <v>847</v>
       </c>
@@ -13188,7 +13190,7 @@
       </c>
       <c r="Q142" s="3"/>
     </row>
-    <row r="143" spans="1:17" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A143" s="19" t="s">
         <v>849</v>
       </c>
@@ -13220,7 +13222,7 @@
         <v>859</v>
       </c>
     </row>
-    <row r="144" spans="1:17" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A144" s="19" t="s">
         <v>851</v>
       </c>
@@ -13252,7 +13254,7 @@
         <v>859</v>
       </c>
     </row>
-    <row r="145" spans="1:17" s="9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:17" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A145" s="6" t="s">
         <v>853</v>
       </c>
@@ -13294,7 +13296,7 @@
       </c>
       <c r="Q145" s="39"/>
     </row>
-    <row r="146" spans="1:17" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:17" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A146" s="19" t="s">
         <v>855</v>
       </c>
@@ -13314,7 +13316,7 @@
         <v>858</v>
       </c>
     </row>
-    <row r="147" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A147" s="19" t="s">
         <v>861</v>
       </c>
@@ -13340,7 +13342,7 @@
         <v>861</v>
       </c>
     </row>
-    <row r="148" spans="1:17" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A148" s="19" t="s">
         <v>863</v>
       </c>
@@ -13369,7 +13371,7 @@
         <v>863</v>
       </c>
     </row>
-    <row r="149" spans="1:17" s="9" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:17" s="9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A149" s="39" t="s">
         <v>14</v>
       </c>
@@ -13416,7 +13418,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="150" spans="1:17" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A150" s="24" t="s">
         <v>25</v>
       </c>
@@ -13454,7 +13456,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="151" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A151" s="8" t="s">
         <v>28</v>
       </c>
@@ -13492,7 +13494,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="152" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A152" s="8" t="s">
         <v>30</v>
       </c>
@@ -13527,7 +13529,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="153" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A153" s="8" t="s">
         <v>31</v>
       </c>
@@ -13565,7 +13567,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="154" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A154" s="8" t="s">
         <v>32</v>
       </c>
@@ -13600,7 +13602,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="155" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A155" s="8" t="s">
         <v>34</v>
       </c>
@@ -13635,7 +13637,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="156" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A156" s="8" t="s">
         <v>37</v>
       </c>
@@ -13673,7 +13675,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="157" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A157" s="8" t="s">
         <v>39</v>
       </c>
@@ -13711,7 +13713,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="158" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A158" s="8" t="s">
         <v>42</v>
       </c>
@@ -13749,7 +13751,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="159" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A159" s="8" t="s">
         <v>43</v>
       </c>
@@ -13787,7 +13789,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="160" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A160" s="8" t="s">
         <v>47</v>
       </c>
@@ -13822,7 +13824,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="161" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A161" s="8" t="s">
         <v>51</v>
       </c>
@@ -13857,7 +13859,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="162" spans="1:17" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A162" s="8" t="s">
         <v>52</v>
       </c>
@@ -13895,7 +13897,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="163" spans="1:17" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A163" s="8" t="s">
         <v>53</v>
       </c>
@@ -13933,7 +13935,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="164" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A164" s="8" t="s">
         <v>54</v>
       </c>
@@ -13971,7 +13973,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="165" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A165" s="8" t="s">
         <v>57</v>
       </c>
@@ -14009,7 +14011,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="166" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A166" s="8" t="s">
         <v>59</v>
       </c>
@@ -14047,7 +14049,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="167" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A167" s="8" t="s">
         <v>60</v>
       </c>
@@ -14085,7 +14087,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="168" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A168" s="8" t="s">
         <v>61</v>
       </c>
@@ -14123,7 +14125,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="169" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A169" s="8" t="s">
         <v>64</v>
       </c>
@@ -14161,7 +14163,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="170" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A170" s="8" t="s">
         <v>69</v>
       </c>
@@ -14199,7 +14201,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="171" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A171" s="8" t="s">
         <v>71</v>
       </c>
@@ -14237,7 +14239,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="172" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A172" s="8" t="s">
         <v>72</v>
       </c>
@@ -14275,7 +14277,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="173" spans="1:17" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A173" s="8" t="s">
         <v>74</v>
       </c>
@@ -14316,7 +14318,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="174" spans="1:17" s="9" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:17" s="9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A174" s="28" t="s">
         <v>75</v>
       </c>
@@ -14364,7 +14366,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="175" spans="1:17" s="9" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:17" s="9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A175" s="8" t="s">
         <v>76</v>
       </c>
@@ -14412,7 +14414,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="176" spans="1:17" s="9" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:17" s="9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A176" s="8" t="s">
         <v>77</v>
       </c>
@@ -14460,7 +14462,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="177" spans="1:17" s="9" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:17" s="9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A177" s="8" t="s">
         <v>78</v>
       </c>
@@ -14508,7 +14510,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="178" spans="1:17" s="9" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:17" s="9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A178" s="3" t="s">
         <v>79</v>
       </c>
@@ -14556,7 +14558,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="179" spans="1:17" s="9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:17" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A179" s="8" t="s">
         <v>80</v>
       </c>
@@ -14603,7 +14605,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="180" spans="1:17" s="9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:17" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A180" s="28" t="s">
         <v>81</v>
       </c>
@@ -14651,7 +14653,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="181" spans="1:17" s="9" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:17" s="9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A181" s="3" t="s">
         <v>82</v>
       </c>
@@ -14699,7 +14701,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="182" spans="1:17" s="9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:17" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A182" s="8" t="s">
         <v>83</v>
       </c>
@@ -14746,7 +14748,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="183" spans="1:17" s="9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:17" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A183" s="28" t="s">
         <v>84</v>
       </c>
@@ -14794,7 +14796,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="184" spans="1:17" s="9" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:17" s="9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A184" s="3" t="s">
         <v>85</v>
       </c>
@@ -14842,7 +14844,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="185" spans="1:17" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A185" s="8" t="s">
         <v>86</v>
       </c>
@@ -14883,7 +14885,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="186" spans="1:17" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A186" s="28" t="s">
         <v>924</v>
       </c>
@@ -14931,7 +14933,7 @@
       </c>
       <c r="Q186" s="28"/>
     </row>
-    <row r="187" spans="1:17" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A187" s="3" t="s">
         <v>924</v>
       </c>
@@ -14979,7 +14981,7 @@
       </c>
       <c r="Q187" s="3"/>
     </row>
-    <row r="188" spans="1:17" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A188" s="8" t="s">
         <v>87</v>
       </c>
@@ -15020,7 +15022,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="189" spans="1:17" s="9" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:17" s="9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A189" s="28" t="s">
         <v>88</v>
       </c>
@@ -15070,7 +15072,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="190" spans="1:17" s="9" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:17" s="9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A190" s="8" t="s">
         <v>89</v>
       </c>
@@ -15118,7 +15120,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="191" spans="1:17" s="9" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:17" s="9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A191" s="16" t="s">
         <v>90</v>
       </c>
@@ -15168,7 +15170,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="192" spans="1:17" s="9" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:17" s="9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A192" s="16" t="s">
         <v>91</v>
       </c>
@@ -15216,7 +15218,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="193" spans="1:17" s="9" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:17" s="9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A193" s="8" t="s">
         <v>92</v>
       </c>
@@ -15264,7 +15266,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="194" spans="1:17" s="9" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:17" s="9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A194" s="8" t="s">
         <v>93</v>
       </c>
@@ -15312,7 +15314,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="195" spans="1:17" s="9" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:17" s="9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A195" s="8" t="s">
         <v>94</v>
       </c>
@@ -15360,7 +15362,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="196" spans="1:17" s="9" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:17" s="9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A196" s="8" t="s">
         <v>95</v>
       </c>
@@ -15408,7 +15410,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="197" spans="1:17" s="9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:17" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A197" s="8" t="s">
         <v>96</v>
       </c>
@@ -15456,7 +15458,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="198" spans="1:17" s="9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:17" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A198" s="8" t="s">
         <v>97</v>
       </c>
@@ -15504,7 +15506,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="199" spans="1:17" s="9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:17" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A199" s="8" t="s">
         <v>98</v>
       </c>
@@ -15552,7 +15554,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="200" spans="1:17" s="9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:17" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A200" s="8" t="s">
         <v>99</v>
       </c>
@@ -15600,7 +15602,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="201" spans="1:17" s="9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:17" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A201" s="16" t="s">
         <v>100</v>
       </c>
@@ -15648,7 +15650,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="202" spans="1:17" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A202" s="8" t="s">
         <v>101</v>
       </c>
@@ -15683,7 +15685,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="203" spans="1:17" s="9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:17" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A203" s="16" t="s">
         <v>102</v>
       </c>
@@ -15731,7 +15733,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="204" spans="1:17" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A204" s="16" t="s">
         <v>103</v>
       </c>
@@ -15779,7 +15781,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="205" spans="1:17" s="9" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:17" s="9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A205" s="16" t="s">
         <v>104</v>
       </c>
@@ -15827,7 +15829,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="206" spans="1:17" s="9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:17" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A206" s="16" t="s">
         <v>105</v>
       </c>
@@ -15877,7 +15879,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="207" spans="1:17" s="9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:17" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A207" s="16" t="s">
         <v>106</v>
       </c>
@@ -15927,7 +15929,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="208" spans="1:17" s="9" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:17" s="9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A208" s="16" t="s">
         <v>107</v>
       </c>
@@ -15977,7 +15979,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="209" spans="1:17" s="9" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:17" s="9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A209" s="16" t="s">
         <v>108</v>
       </c>
@@ -16027,7 +16029,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="210" spans="1:17" s="9" customFormat="1" ht="56.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:17" s="9" customFormat="1" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A210" s="16" t="s">
         <v>109</v>
       </c>
@@ -16077,7 +16079,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="211" spans="1:17" s="9" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:17" s="9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A211" s="3" t="s">
         <v>110</v>
       </c>
@@ -16127,7 +16129,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="212" spans="1:17" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A212" s="8" t="s">
         <v>111</v>
       </c>
@@ -16162,7 +16164,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="213" spans="1:17" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A213" s="8" t="s">
         <v>112</v>
       </c>
@@ -16197,7 +16199,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="214" spans="1:17" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A214" s="8" t="s">
         <v>114</v>
       </c>
@@ -16235,7 +16237,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="215" spans="1:17" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A215" s="8" t="s">
         <v>115</v>
       </c>
@@ -16273,7 +16275,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="216" spans="1:17" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A216" s="8" t="s">
         <v>116</v>
       </c>
@@ -16311,7 +16313,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="217" spans="1:17" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A217" s="8" t="s">
         <v>117</v>
       </c>
@@ -16346,7 +16348,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="218" spans="1:17" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A218" s="8" t="s">
         <v>118</v>
       </c>
@@ -16381,7 +16383,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="219" spans="1:17" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A219" s="8" t="s">
         <v>119</v>
       </c>
@@ -16416,7 +16418,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="220" spans="1:17" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A220" s="8" t="s">
         <v>120</v>
       </c>
@@ -16454,7 +16456,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="221" spans="1:17" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A221" s="8" t="s">
         <v>121</v>
       </c>
@@ -16489,7 +16491,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="222" spans="1:17" ht="147" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:17" ht="147" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A222" s="8" t="s">
         <v>122</v>
       </c>
@@ -16527,7 +16529,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="223" spans="1:17" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A223" s="8" t="s">
         <v>123</v>
       </c>
@@ -16562,7 +16564,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="224" spans="1:17" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A224" s="8" t="s">
         <v>124</v>
       </c>
@@ -16597,7 +16599,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="225" spans="1:17" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A225" s="8" t="s">
         <v>126</v>
       </c>
@@ -16635,7 +16637,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="226" spans="1:17" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A226" s="8" t="s">
         <v>127</v>
       </c>
@@ -16673,7 +16675,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="227" spans="1:17" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A227" s="16" t="s">
         <v>128</v>
       </c>
@@ -16723,7 +16725,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="228" spans="1:17" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A228" s="16" t="s">
         <v>1662</v>
       </c>
@@ -16773,7 +16775,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="229" spans="1:17" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A229" s="3" t="s">
         <v>132</v>
       </c>
@@ -16824,7 +16826,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="230" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A230" s="8" t="s">
         <v>133</v>
       </c>
@@ -16865,7 +16867,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="231" spans="1:17" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A231" s="39" t="s">
         <v>134</v>
       </c>
@@ -16914,7 +16916,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="232" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A232" s="8" t="s">
         <v>135</v>
       </c>
@@ -16952,7 +16954,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="233" spans="1:17" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A233" s="16" t="s">
         <v>136</v>
       </c>
@@ -17002,7 +17004,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="234" spans="1:17" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A234" s="16" t="s">
         <v>138</v>
       </c>
@@ -17052,7 +17054,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="235" spans="1:17" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A235" s="16" t="s">
         <v>139</v>
       </c>
@@ -17102,7 +17104,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="236" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A236" s="8" t="s">
         <v>142</v>
       </c>
@@ -17140,7 +17142,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="237" spans="1:17" s="9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:17" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A237" s="17" t="s">
         <v>648</v>
       </c>
@@ -17187,7 +17189,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="238" spans="1:17" s="9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:17" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A238" s="17" t="s">
         <v>578</v>
       </c>
@@ -17234,7 +17236,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="239" spans="1:17" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A239" s="24" t="s">
         <v>604</v>
       </c>
@@ -17272,7 +17274,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="240" spans="1:17" s="9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:17" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A240" s="17" t="s">
         <v>602</v>
       </c>
@@ -17316,7 +17318,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="241" spans="1:17" s="9" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:17" s="9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A241" s="17" t="s">
         <v>608</v>
       </c>
@@ -17360,7 +17362,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="242" spans="1:17" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A242" s="8" t="s">
         <v>150</v>
       </c>
@@ -17398,7 +17400,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="243" spans="1:17" s="9" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:17" s="9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A243" s="17" t="s">
         <v>612</v>
       </c>
@@ -17445,7 +17447,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="244" spans="1:17" s="9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:17" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A244" s="17" t="s">
         <v>606</v>
       </c>
@@ -17489,7 +17491,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="245" spans="1:17" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:17" ht="60" x14ac:dyDescent="0.25">
       <c r="A245" s="8" t="s">
         <v>169</v>
       </c>
@@ -17524,7 +17526,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="246" spans="1:17" s="9" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:17" s="9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A246" s="17" t="s">
         <v>610</v>
       </c>
@@ -17566,7 +17568,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="247" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A247" s="8" t="s">
         <v>171</v>
       </c>
@@ -17601,7 +17603,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="248" spans="1:17" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A248" s="24" t="s">
         <v>522</v>
       </c>
@@ -17633,7 +17635,7 @@
         <v>1426</v>
       </c>
     </row>
-    <row r="249" spans="1:17" s="9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:17" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A249" s="17" t="s">
         <v>588</v>
       </c>
@@ -17680,7 +17682,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="250" spans="1:17" s="9" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:17" s="9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A250" s="17" t="s">
         <v>590</v>
       </c>
@@ -17727,7 +17729,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="251" spans="1:17" s="9" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:17" s="9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A251" s="16" t="s">
         <v>143</v>
       </c>
@@ -17777,7 +17779,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="252" spans="1:17" s="9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:17" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A252" s="17" t="s">
         <v>586</v>
       </c>
@@ -17824,7 +17826,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="253" spans="1:17" s="9" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:17" s="9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A253" s="17" t="s">
         <v>592</v>
       </c>
@@ -17871,7 +17873,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="254" spans="1:17" s="9" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:17" s="9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A254" s="17" t="s">
         <v>594</v>
       </c>
@@ -17918,7 +17920,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="255" spans="1:17" s="9" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:17" s="9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A255" s="17" t="s">
         <v>596</v>
       </c>
@@ -17965,7 +17967,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="256" spans="1:17" s="9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:17" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A256" s="17" t="s">
         <v>598</v>
       </c>
@@ -18012,7 +18014,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="257" spans="1:17" s="9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:17" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A257" s="17" t="s">
         <v>600</v>
       </c>
@@ -18059,7 +18061,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="258" spans="1:17" s="9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:17" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A258" s="16" t="s">
         <v>144</v>
       </c>
@@ -18109,7 +18111,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="259" spans="1:17" s="9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:17" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A259" s="16" t="s">
         <v>170</v>
       </c>
@@ -18159,7 +18161,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="260" spans="1:17" s="9" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:17" s="9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A260" s="17" t="s">
         <v>584</v>
       </c>
@@ -18206,7 +18208,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="261" spans="1:17" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A261" s="24" t="s">
         <v>526</v>
       </c>
@@ -18247,7 +18249,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="262" spans="1:17" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A262" s="24" t="s">
         <v>528</v>
       </c>
@@ -18288,7 +18290,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="263" spans="1:17" s="9" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:17" s="9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A263" s="17" t="s">
         <v>566</v>
       </c>
@@ -18335,7 +18337,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="264" spans="1:17" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A264" s="24" t="s">
         <v>532</v>
       </c>
@@ -18373,7 +18375,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="265" spans="1:17" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A265" s="24" t="s">
         <v>534</v>
       </c>
@@ -18414,7 +18416,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="266" spans="1:17" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A266" s="24" t="s">
         <v>536</v>
       </c>
@@ -18455,7 +18457,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="267" spans="1:17" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A267" s="24" t="s">
         <v>538</v>
       </c>
@@ -18496,7 +18498,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="268" spans="1:17" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A268" s="24" t="s">
         <v>540</v>
       </c>
@@ -18537,7 +18539,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="269" spans="1:17" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A269" s="24" t="s">
         <v>542</v>
       </c>
@@ -18578,7 +18580,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="270" spans="1:17" s="9" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:17" s="9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A270" s="17" t="s">
         <v>568</v>
       </c>
@@ -18625,7 +18627,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="271" spans="1:17" s="9" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:17" s="9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A271" s="17" t="s">
         <v>570</v>
       </c>
@@ -18672,7 +18674,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="272" spans="1:17" s="9" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:17" s="9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A272" s="17" t="s">
         <v>572</v>
       </c>
@@ -18719,7 +18721,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="273" spans="1:17" s="9" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:17" s="9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A273" s="24" t="s">
         <v>574</v>
       </c>
@@ -18766,7 +18768,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="274" spans="1:17" s="9" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:17" s="9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A274" s="17" t="s">
         <v>576</v>
       </c>
@@ -18813,7 +18815,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="275" spans="1:17" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A275" s="24" t="s">
         <v>630</v>
       </c>
@@ -18854,7 +18856,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="276" spans="1:17" s="9" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:17" s="9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A276" s="17" t="s">
         <v>632</v>
       </c>
@@ -18901,7 +18903,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="277" spans="1:17" s="9" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:17" s="9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A277" s="17" t="s">
         <v>634</v>
       </c>
@@ -18948,7 +18950,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="278" spans="1:17" s="9" customFormat="1" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:17" s="9" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A278" s="17" t="s">
         <v>636</v>
       </c>
@@ -18995,7 +18997,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="279" spans="1:17" s="9" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:17" s="9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A279" s="17" t="s">
         <v>638</v>
       </c>
@@ -19042,7 +19044,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="280" spans="1:17" s="9" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:17" s="9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A280" s="17" t="s">
         <v>640</v>
       </c>
@@ -19089,7 +19091,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="281" spans="1:17" s="9" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:17" s="9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A281" s="17" t="s">
         <v>642</v>
       </c>
@@ -19136,7 +19138,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="282" spans="1:17" s="9" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:17" s="9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A282" s="17" t="s">
         <v>644</v>
       </c>
@@ -19183,7 +19185,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="283" spans="1:17" s="9" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:17" s="9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A283" s="17" t="s">
         <v>646</v>
       </c>
@@ -19230,7 +19232,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="284" spans="1:17" s="9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:17" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A284" s="17" t="s">
         <v>544</v>
       </c>
@@ -19277,7 +19279,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="285" spans="1:17" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A285" s="24" t="s">
         <v>546</v>
       </c>
@@ -19315,7 +19317,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="286" spans="1:17" s="9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:17" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A286" s="17" t="s">
         <v>548</v>
       </c>
@@ -19362,7 +19364,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="287" spans="1:17" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A287" s="24" t="s">
         <v>550</v>
       </c>
@@ -19403,7 +19405,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="288" spans="1:17" s="9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:17" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A288" s="17" t="s">
         <v>552</v>
       </c>
@@ -19450,7 +19452,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="289" spans="1:17" s="9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:17" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A289" s="17" t="s">
         <v>554</v>
       </c>
@@ -19497,7 +19499,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="290" spans="1:17" s="9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:17" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A290" s="17" t="s">
         <v>556</v>
       </c>
@@ -19544,7 +19546,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="291" spans="1:17" s="9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:17" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A291" s="24" t="s">
         <v>558</v>
       </c>
@@ -19591,7 +19593,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="292" spans="1:17" s="9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:17" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A292" s="17" t="s">
         <v>560</v>
       </c>
@@ -19638,7 +19640,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="293" spans="1:17" s="9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:17" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A293" s="16" t="s">
         <v>149</v>
       </c>
@@ -19685,7 +19687,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="294" spans="1:17" s="9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:17" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A294" s="17" t="s">
         <v>616</v>
       </c>
@@ -19729,7 +19731,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="295" spans="1:17" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A295" s="24" t="s">
         <v>620</v>
       </c>
@@ -19764,7 +19766,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="296" spans="1:17" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A296" s="8" t="s">
         <v>146</v>
       </c>
@@ -19805,7 +19807,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="297" spans="1:17" s="9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:17" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A297" s="16" t="s">
         <v>147</v>
       </c>
@@ -19855,7 +19857,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="298" spans="1:17" s="9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:17" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A298" s="16" t="s">
         <v>148</v>
       </c>
@@ -19905,7 +19907,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="299" spans="1:17" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A299" s="24" t="s">
         <v>614</v>
       </c>
@@ -19943,7 +19945,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="300" spans="1:17" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A300" s="24" t="s">
         <v>618</v>
       </c>
@@ -19981,7 +19983,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="301" spans="1:17" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A301" s="24" t="s">
         <v>622</v>
       </c>
@@ -20019,7 +20021,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="302" spans="1:17" s="9" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:17" s="9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A302" s="17" t="s">
         <v>624</v>
       </c>
@@ -20063,7 +20065,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="303" spans="1:17" s="9" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:17" s="9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A303" s="17" t="s">
         <v>626</v>
       </c>
@@ -20107,7 +20109,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="304" spans="1:17" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A304" s="24" t="s">
         <v>628</v>
       </c>
@@ -20142,7 +20144,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="305" spans="1:17" ht="197.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:17" ht="197.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A305" s="24" t="s">
         <v>582</v>
       </c>
@@ -20183,7 +20185,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="306" spans="1:17" s="9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:17" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A306" s="79" t="s">
         <v>580</v>
       </c>
@@ -20230,7 +20232,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="307" spans="1:17" s="9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:17" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A307" s="83" t="s">
         <v>564</v>
       </c>
@@ -20271,7 +20273,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="308" spans="1:17" s="9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:17" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A308" s="17" t="s">
         <v>562</v>
       </c>
@@ -20318,7 +20320,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="309" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A309" s="24" t="s">
         <v>530</v>
       </c>
@@ -20359,7 +20361,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="310" spans="1:17" s="9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:17" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A310" s="14" t="s">
         <v>952</v>
       </c>
@@ -20403,7 +20405,7 @@
         <v>952</v>
       </c>
     </row>
-    <row r="311" spans="1:17" s="9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:17" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A311" s="14" t="s">
         <v>956</v>
       </c>
@@ -20447,7 +20449,7 @@
         <v>956</v>
       </c>
     </row>
-    <row r="312" spans="1:17" s="9" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:17" s="9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A312" s="14" t="s">
         <v>960</v>
       </c>
@@ -20491,7 +20493,7 @@
         <v>960</v>
       </c>
     </row>
-    <row r="313" spans="1:17" ht="390" hidden="1" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:17" ht="390" x14ac:dyDescent="0.25">
       <c r="A313" s="32" t="s">
         <v>967</v>
       </c>
@@ -20532,7 +20534,7 @@
         <v>971</v>
       </c>
     </row>
-    <row r="314" spans="1:17" s="9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:17" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A314" s="21" t="s">
         <v>973</v>
       </c>
@@ -20576,7 +20578,7 @@
         <v>973</v>
       </c>
     </row>
-    <row r="315" spans="1:17" s="9" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:17" s="9" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A315" s="14" t="s">
         <v>976</v>
       </c>
@@ -20621,7 +20623,7 @@
         <v>976</v>
       </c>
     </row>
-    <row r="316" spans="1:17" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:17" ht="60" x14ac:dyDescent="0.25">
       <c r="A316" s="19" t="s">
         <v>981</v>
       </c>
@@ -20656,7 +20658,7 @@
         <v>981</v>
       </c>
     </row>
-    <row r="317" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A317" s="19" t="s">
         <v>984</v>
       </c>
@@ -20691,7 +20693,7 @@
         <v>984</v>
       </c>
     </row>
-    <row r="318" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A318" s="19" t="s">
         <v>987</v>
       </c>
@@ -20714,7 +20716,7 @@
         <v>1062</v>
       </c>
     </row>
-    <row r="319" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A319" s="60" t="s">
         <v>989</v>
       </c>
@@ -20737,7 +20739,7 @@
         <v>1062</v>
       </c>
     </row>
-    <row r="320" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A320" s="19" t="s">
         <v>991</v>
       </c>
@@ -20760,7 +20762,7 @@
         <v>1062</v>
       </c>
     </row>
-    <row r="321" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A321" s="19" t="s">
         <v>993</v>
       </c>
@@ -20792,7 +20794,7 @@
         <v>993</v>
       </c>
     </row>
-    <row r="322" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A322" s="19" t="s">
         <v>995</v>
       </c>
@@ -20821,7 +20823,7 @@
         <v>995</v>
       </c>
     </row>
-    <row r="323" spans="1:17" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A323" s="21" t="s">
         <v>997</v>
       </c>
@@ -20862,7 +20864,7 @@
         <v>997</v>
       </c>
     </row>
-    <row r="324" spans="1:17" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A324" s="6" t="s">
         <v>999</v>
       </c>
@@ -20903,7 +20905,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="325" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A325" s="19" t="s">
         <v>1001</v>
       </c>
@@ -20932,7 +20934,7 @@
         <v>1001</v>
       </c>
     </row>
-    <row r="326" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A326" s="19" t="s">
         <v>1003</v>
       </c>
@@ -20961,7 +20963,7 @@
         <v>1003</v>
       </c>
     </row>
-    <row r="327" spans="1:17" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A327" s="35" t="s">
         <v>1005</v>
       </c>
@@ -21006,7 +21008,7 @@
       <c r="P327" s="39"/>
       <c r="Q327" s="39"/>
     </row>
-    <row r="328" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A328" s="19" t="s">
         <v>1007</v>
       </c>
@@ -21035,7 +21037,7 @@
         <v>1007</v>
       </c>
     </row>
-    <row r="329" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A329" s="19" t="s">
         <v>1009</v>
       </c>
@@ -21064,7 +21066,7 @@
         <v>1009</v>
       </c>
     </row>
-    <row r="330" spans="1:17" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A330" s="21" t="s">
         <v>1011</v>
       </c>
@@ -21105,7 +21107,7 @@
         <v>1011</v>
       </c>
     </row>
-    <row r="331" spans="1:17" s="9" customFormat="1" ht="135" hidden="1" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:17" s="9" customFormat="1" ht="135" x14ac:dyDescent="0.25">
       <c r="A331" s="6" t="s">
         <v>1014</v>
       </c>
@@ -21152,7 +21154,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="332" spans="1:17" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A332" s="33" t="s">
         <v>1017</v>
       </c>
@@ -21195,7 +21197,7 @@
       <c r="P332" s="8"/>
       <c r="Q332" s="8"/>
     </row>
-    <row r="333" spans="1:17" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A333" s="19" t="s">
         <v>1019</v>
       </c>
@@ -21234,7 +21236,7 @@
       <c r="P333" s="8"/>
       <c r="Q333" s="8"/>
     </row>
-    <row r="334" spans="1:17" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A334" s="9" t="s">
         <v>1021</v>
       </c>
@@ -21272,7 +21274,7 @@
         <v>1021</v>
       </c>
     </row>
-    <row r="335" spans="1:17" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A335" s="6" t="s">
         <v>1023</v>
       </c>
@@ -21313,7 +21315,7 @@
         <v>1023</v>
       </c>
     </row>
-    <row r="336" spans="1:17" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A336" s="6" t="s">
         <v>1025</v>
       </c>
@@ -21354,7 +21356,7 @@
         <v>1023</v>
       </c>
     </row>
-    <row r="337" spans="1:15" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A337" s="6" t="s">
         <v>1027</v>
       </c>
@@ -21395,7 +21397,7 @@
         <v>1023</v>
       </c>
     </row>
-    <row r="338" spans="1:15" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A338" s="6" t="s">
         <v>1029</v>
       </c>
@@ -21436,7 +21438,7 @@
         <v>1023</v>
       </c>
     </row>
-    <row r="339" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A339" s="19" t="s">
         <v>1032</v>
       </c>
@@ -21465,7 +21467,7 @@
         <v>1033</v>
       </c>
     </row>
-    <row r="340" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A340" s="19" t="s">
         <v>1034</v>
       </c>
@@ -21494,7 +21496,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="341" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A341" s="19" t="s">
         <v>1036</v>
       </c>
@@ -21523,7 +21525,7 @@
         <v>1037</v>
       </c>
     </row>
-    <row r="342" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A342" s="19" t="s">
         <v>1038</v>
       </c>
@@ -21552,7 +21554,7 @@
         <v>1039</v>
       </c>
     </row>
-    <row r="343" spans="1:15" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A343" s="6" t="s">
         <v>1064</v>
       </c>
@@ -21593,7 +21595,7 @@
         <v>1064</v>
       </c>
     </row>
-    <row r="344" spans="1:15" s="9" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:15" s="9" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A344" s="6" t="s">
         <v>1068</v>
       </c>
@@ -21637,7 +21639,7 @@
         <v>1068</v>
       </c>
     </row>
-    <row r="345" spans="1:15" ht="120" hidden="1" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:15" ht="120" x14ac:dyDescent="0.25">
       <c r="A345" s="19" t="s">
         <v>1073</v>
       </c>
@@ -21669,7 +21671,7 @@
         <v>1073</v>
       </c>
     </row>
-    <row r="346" spans="1:15" ht="195" hidden="1" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:15" ht="195" x14ac:dyDescent="0.25">
       <c r="A346" s="19" t="s">
         <v>1077</v>
       </c>
@@ -21701,7 +21703,7 @@
         <v>1073</v>
       </c>
     </row>
-    <row r="347" spans="1:15" s="9" customFormat="1" ht="51.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:15" s="9" customFormat="1" ht="51.75" x14ac:dyDescent="0.25">
       <c r="A347" s="14" t="s">
         <v>1082</v>
       </c>
@@ -21745,7 +21747,7 @@
         <v>1082</v>
       </c>
     </row>
-    <row r="348" spans="1:15" ht="135" hidden="1" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:15" ht="135" x14ac:dyDescent="0.25">
       <c r="A348" s="12" t="s">
         <v>1086</v>
       </c>
@@ -21783,7 +21785,7 @@
         <v>1086</v>
       </c>
     </row>
-    <row r="349" spans="1:15" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:15" ht="150" x14ac:dyDescent="0.25">
       <c r="A349" s="32" t="s">
         <v>1093</v>
       </c>
@@ -21818,7 +21820,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="350" spans="1:15" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:15" ht="165" x14ac:dyDescent="0.25">
       <c r="A350" s="32" t="s">
         <v>1096</v>
       </c>
@@ -21853,7 +21855,7 @@
         <v>1096</v>
       </c>
     </row>
-    <row r="351" spans="1:15" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A351" s="8" t="s">
         <v>1105</v>
       </c>
@@ -21885,7 +21887,7 @@
         <v>1105</v>
       </c>
     </row>
-    <row r="352" spans="1:15" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A352" s="19" t="s">
         <v>1101</v>
       </c>
@@ -21920,7 +21922,7 @@
         <v>1101</v>
       </c>
     </row>
-    <row r="353" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A353" s="19" t="s">
         <v>1108</v>
       </c>
@@ -21955,7 +21957,7 @@
         <v>1108</v>
       </c>
     </row>
-    <row r="354" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A354" s="19" t="s">
         <v>1110</v>
       </c>
@@ -21990,7 +21992,7 @@
         <v>1108</v>
       </c>
     </row>
-    <row r="355" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A355" s="19" t="s">
         <v>1112</v>
       </c>
@@ -22025,7 +22027,7 @@
         <v>1108</v>
       </c>
     </row>
-    <row r="356" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A356" s="19" t="s">
         <v>1114</v>
       </c>
@@ -22060,7 +22062,7 @@
         <v>1108</v>
       </c>
     </row>
-    <row r="357" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A357" s="19" t="s">
         <v>1116</v>
       </c>
@@ -22095,7 +22097,7 @@
         <v>1108</v>
       </c>
     </row>
-    <row r="358" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A358" s="19" t="s">
         <v>1118</v>
       </c>
@@ -22130,7 +22132,7 @@
         <v>1108</v>
       </c>
     </row>
-    <row r="359" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A359" s="19" t="s">
         <v>1120</v>
       </c>
@@ -22165,7 +22167,7 @@
         <v>1108</v>
       </c>
     </row>
-    <row r="360" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A360" s="19" t="s">
         <v>1122</v>
       </c>
@@ -22200,7 +22202,7 @@
         <v>1108</v>
       </c>
     </row>
-    <row r="361" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A361" s="19" t="s">
         <v>1124</v>
       </c>
@@ -22235,7 +22237,7 @@
         <v>1108</v>
       </c>
     </row>
-    <row r="362" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A362" s="19" t="s">
         <v>1126</v>
       </c>
@@ -22270,7 +22272,7 @@
         <v>1108</v>
       </c>
     </row>
-    <row r="363" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A363" s="19" t="s">
         <v>1129</v>
       </c>
@@ -22305,7 +22307,7 @@
         <v>1129</v>
       </c>
     </row>
-    <row r="364" spans="1:15" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A364" s="19" t="s">
         <v>1131</v>
       </c>
@@ -22340,7 +22342,7 @@
         <v>1129</v>
       </c>
     </row>
-    <row r="365" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A365" s="19" t="s">
         <v>1133</v>
       </c>
@@ -22375,7 +22377,7 @@
         <v>1129</v>
       </c>
     </row>
-    <row r="366" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A366" s="19" t="s">
         <v>1135</v>
       </c>
@@ -22410,7 +22412,7 @@
         <v>1129</v>
       </c>
     </row>
-    <row r="367" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A367" s="19" t="s">
         <v>1137</v>
       </c>
@@ -22445,7 +22447,7 @@
         <v>1129</v>
       </c>
     </row>
-    <row r="368" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A368" s="19" t="s">
         <v>1139</v>
       </c>
@@ -22480,7 +22482,7 @@
         <v>1129</v>
       </c>
     </row>
-    <row r="369" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A369" s="19" t="s">
         <v>1141</v>
       </c>
@@ -22515,7 +22517,7 @@
         <v>1129</v>
       </c>
     </row>
-    <row r="370" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A370" s="19" t="s">
         <v>1143</v>
       </c>
@@ -22550,7 +22552,7 @@
         <v>1129</v>
       </c>
     </row>
-    <row r="371" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A371" s="19" t="s">
         <v>1145</v>
       </c>
@@ -22585,7 +22587,7 @@
         <v>1129</v>
       </c>
     </row>
-    <row r="372" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A372" s="19" t="s">
         <v>1147</v>
       </c>
@@ -22620,7 +22622,7 @@
         <v>1129</v>
       </c>
     </row>
-    <row r="373" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A373" s="19" t="s">
         <v>1149</v>
       </c>
@@ -22655,7 +22657,7 @@
         <v>1129</v>
       </c>
     </row>
-    <row r="374" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A374" s="19" t="s">
         <v>1151</v>
       </c>
@@ -22690,7 +22692,7 @@
         <v>1129</v>
       </c>
     </row>
-    <row r="375" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A375" s="19" t="s">
         <v>1153</v>
       </c>
@@ -22725,7 +22727,7 @@
         <v>1129</v>
       </c>
     </row>
-    <row r="376" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A376" s="19" t="s">
         <v>1155</v>
       </c>
@@ -22760,7 +22762,7 @@
         <v>1129</v>
       </c>
     </row>
-    <row r="377" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A377" s="19" t="s">
         <v>1157</v>
       </c>
@@ -22795,7 +22797,7 @@
         <v>1129</v>
       </c>
     </row>
-    <row r="378" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A378" s="19" t="s">
         <v>1159</v>
       </c>
@@ -22830,7 +22832,7 @@
         <v>1129</v>
       </c>
     </row>
-    <row r="379" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A379" s="19" t="s">
         <v>1161</v>
       </c>
@@ -22865,7 +22867,7 @@
         <v>1129</v>
       </c>
     </row>
-    <row r="380" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A380" s="19" t="s">
         <v>1163</v>
       </c>
@@ -22900,7 +22902,7 @@
         <v>1129</v>
       </c>
     </row>
-    <row r="381" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="381" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A381" s="19" t="s">
         <v>1165</v>
       </c>
@@ -22935,7 +22937,7 @@
         <v>1129</v>
       </c>
     </row>
-    <row r="382" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="382" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A382" s="19" t="s">
         <v>1167</v>
       </c>
@@ -22970,7 +22972,7 @@
         <v>1129</v>
       </c>
     </row>
-    <row r="383" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="383" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A383" s="19" t="s">
         <v>1169</v>
       </c>
@@ -23005,7 +23007,7 @@
         <v>1129</v>
       </c>
     </row>
-    <row r="384" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="384" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A384" s="19" t="s">
         <v>1172</v>
       </c>
@@ -23040,7 +23042,7 @@
         <v>1172</v>
       </c>
     </row>
-    <row r="385" spans="1:15" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="385" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A385" s="6" t="s">
         <v>1175</v>
       </c>
@@ -23084,7 +23086,7 @@
         <v>1226</v>
       </c>
     </row>
-    <row r="386" spans="1:15" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="386" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A386" s="6" t="s">
         <v>1177</v>
       </c>
@@ -23128,7 +23130,7 @@
         <v>1226</v>
       </c>
     </row>
-    <row r="387" spans="1:15" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="387" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A387" s="6" t="s">
         <v>1179</v>
       </c>
@@ -23172,7 +23174,7 @@
         <v>1226</v>
       </c>
     </row>
-    <row r="388" spans="1:15" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="388" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A388" s="6" t="s">
         <v>1181</v>
       </c>
@@ -23216,7 +23218,7 @@
         <v>1226</v>
       </c>
     </row>
-    <row r="389" spans="1:15" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="389" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A389" s="6" t="s">
         <v>1183</v>
       </c>
@@ -23260,7 +23262,7 @@
         <v>1226</v>
       </c>
     </row>
-    <row r="390" spans="1:15" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="390" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A390" s="6" t="s">
         <v>1185</v>
       </c>
@@ -23304,7 +23306,7 @@
         <v>1226</v>
       </c>
     </row>
-    <row r="391" spans="1:15" s="9" customFormat="1" ht="209.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="391" spans="1:15" s="9" customFormat="1" ht="209.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A391" s="6" t="s">
         <v>1187</v>
       </c>
@@ -23348,7 +23350,7 @@
         <v>1226</v>
       </c>
     </row>
-    <row r="392" spans="1:15" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="392" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A392" s="6" t="s">
         <v>1189</v>
       </c>
@@ -23392,7 +23394,7 @@
         <v>1226</v>
       </c>
     </row>
-    <row r="393" spans="1:15" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="393" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A393" s="6" t="s">
         <v>1191</v>
       </c>
@@ -23434,7 +23436,7 @@
         <v>1226</v>
       </c>
     </row>
-    <row r="394" spans="1:15" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="394" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A394" s="6" t="s">
         <v>1193</v>
       </c>
@@ -23478,7 +23480,7 @@
         <v>1226</v>
       </c>
     </row>
-    <row r="395" spans="1:15" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="395" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A395" s="6" t="s">
         <v>1195</v>
       </c>
@@ -23522,7 +23524,7 @@
         <v>1226</v>
       </c>
     </row>
-    <row r="396" spans="1:15" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="396" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A396" s="21" t="s">
         <v>1197</v>
       </c>
@@ -23566,7 +23568,7 @@
         <v>1226</v>
       </c>
     </row>
-    <row r="397" spans="1:15" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="397" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A397" s="6" t="s">
         <v>1199</v>
       </c>
@@ -23610,7 +23612,7 @@
         <v>1226</v>
       </c>
     </row>
-    <row r="398" spans="1:15" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="398" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A398" s="19" t="s">
         <v>1201</v>
       </c>
@@ -23654,7 +23656,7 @@
         <v>1226</v>
       </c>
     </row>
-    <row r="399" spans="1:15" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="399" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A399" s="19" t="s">
         <v>1203</v>
       </c>
@@ -23698,7 +23700,7 @@
         <v>1226</v>
       </c>
     </row>
-    <row r="400" spans="1:15" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="400" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A400" s="19" t="s">
         <v>1205</v>
       </c>
@@ -23740,7 +23742,7 @@
         <v>1226</v>
       </c>
     </row>
-    <row r="401" spans="1:15" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="401" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A401" s="19" t="s">
         <v>1177</v>
       </c>
@@ -23784,7 +23786,7 @@
         <v>1226</v>
       </c>
     </row>
-    <row r="402" spans="1:15" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="402" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A402" s="19" t="s">
         <v>1189</v>
       </c>
@@ -23828,7 +23830,7 @@
         <v>1226</v>
       </c>
     </row>
-    <row r="403" spans="1:15" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="403" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A403" s="48" t="s">
         <v>1203</v>
       </c>
@@ -23872,7 +23874,7 @@
         <v>1226</v>
       </c>
     </row>
-    <row r="404" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="404" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A404" s="19" t="s">
         <v>1207</v>
       </c>
@@ -23907,7 +23909,7 @@
         <v>1226</v>
       </c>
     </row>
-    <row r="405" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="405" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A405" s="19" t="s">
         <v>1209</v>
       </c>
@@ -23942,7 +23944,7 @@
         <v>1226</v>
       </c>
     </row>
-    <row r="406" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="406" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A406" s="19" t="s">
         <v>1227</v>
       </c>
@@ -23974,7 +23976,7 @@
         <v>1227</v>
       </c>
     </row>
-    <row r="407" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="407" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A407" s="19" t="s">
         <v>1229</v>
       </c>
@@ -24006,7 +24008,7 @@
         <v>1274</v>
       </c>
     </row>
-    <row r="408" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="408" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A408" s="19" t="s">
         <v>1231</v>
       </c>
@@ -24038,7 +24040,7 @@
         <v>1227</v>
       </c>
     </row>
-    <row r="409" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="409" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A409" s="19" t="s">
         <v>1233</v>
       </c>
@@ -24070,7 +24072,7 @@
         <v>1227</v>
       </c>
     </row>
-    <row r="410" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="410" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A410" s="19" t="s">
         <v>1235</v>
       </c>
@@ -24102,7 +24104,7 @@
         <v>1227</v>
       </c>
     </row>
-    <row r="411" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="411" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A411" s="19" t="s">
         <v>1237</v>
       </c>
@@ -24134,7 +24136,7 @@
         <v>1227</v>
       </c>
     </row>
-    <row r="412" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="412" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A412" s="19" t="s">
         <v>1239</v>
       </c>
@@ -24166,7 +24168,7 @@
         <v>1227</v>
       </c>
     </row>
-    <row r="413" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="413" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A413" s="19" t="s">
         <v>1241</v>
       </c>
@@ -24198,7 +24200,7 @@
         <v>1227</v>
       </c>
     </row>
-    <row r="414" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="414" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A414" s="19" t="s">
         <v>1243</v>
       </c>
@@ -24230,7 +24232,7 @@
         <v>1227</v>
       </c>
     </row>
-    <row r="415" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="415" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A415" s="19" t="s">
         <v>1245</v>
       </c>
@@ -24262,7 +24264,7 @@
         <v>1227</v>
       </c>
     </row>
-    <row r="416" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="416" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A416" s="19" t="s">
         <v>1247</v>
       </c>
@@ -24294,7 +24296,7 @@
         <v>1227</v>
       </c>
     </row>
-    <row r="417" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="417" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A417" s="19" t="s">
         <v>1249</v>
       </c>
@@ -24326,7 +24328,7 @@
         <v>1270</v>
       </c>
     </row>
-    <row r="418" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="418" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A418" s="19" t="s">
         <v>1251</v>
       </c>
@@ -24358,7 +24360,7 @@
         <v>1227</v>
       </c>
     </row>
-    <row r="419" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="419" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A419" s="19" t="s">
         <v>1253</v>
       </c>
@@ -24390,7 +24392,7 @@
         <v>1269</v>
       </c>
     </row>
-    <row r="420" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="420" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A420" s="19" t="s">
         <v>1255</v>
       </c>
@@ -24422,7 +24424,7 @@
         <v>1227</v>
       </c>
     </row>
-    <row r="421" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="421" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A421" s="19" t="s">
         <v>1257</v>
       </c>
@@ -24454,7 +24456,7 @@
         <v>1227</v>
       </c>
     </row>
-    <row r="422" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="422" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A422" s="19" t="s">
         <v>1259</v>
       </c>
@@ -24486,7 +24488,7 @@
         <v>1227</v>
       </c>
     </row>
-    <row r="423" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="423" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A423" s="19" t="s">
         <v>1261</v>
       </c>
@@ -24518,7 +24520,7 @@
         <v>1227</v>
       </c>
     </row>
-    <row r="424" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="424" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A424" s="19" t="s">
         <v>1263</v>
       </c>
@@ -24550,7 +24552,7 @@
         <v>1227</v>
       </c>
     </row>
-    <row r="425" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="425" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A425" s="19" t="s">
         <v>1272</v>
       </c>
@@ -24582,7 +24584,7 @@
         <v>1273</v>
       </c>
     </row>
-    <row r="426" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="426" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A426" s="19" t="s">
         <v>1265</v>
       </c>
@@ -24614,7 +24616,7 @@
         <v>1227</v>
       </c>
     </row>
-    <row r="427" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="427" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A427" s="19" t="s">
         <v>1267</v>
       </c>
@@ -24652,7 +24654,7 @@
         <v>1227</v>
       </c>
     </row>
-    <row r="428" spans="1:15" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="428" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A428" s="86" t="s">
         <v>1275</v>
       </c>
@@ -24696,7 +24698,7 @@
         <v>1275</v>
       </c>
     </row>
-    <row r="429" spans="1:15" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="429" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A429" s="48" t="s">
         <v>1277</v>
       </c>
@@ -24740,7 +24742,7 @@
         <v>1277</v>
       </c>
     </row>
-    <row r="430" spans="1:15" ht="315" hidden="1" x14ac:dyDescent="0.25">
+    <row r="430" spans="1:15" ht="315" x14ac:dyDescent="0.25">
       <c r="A430" s="32" t="s">
         <v>1422</v>
       </c>
@@ -24778,7 +24780,7 @@
         <v>1283</v>
       </c>
     </row>
-    <row r="431" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="431" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A431" s="19" t="s">
         <v>1285</v>
       </c>
@@ -24810,7 +24812,7 @@
         <v>1285</v>
       </c>
     </row>
-    <row r="432" spans="1:15" ht="409.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="432" spans="1:15" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A432" s="19" t="s">
         <v>1287</v>
       </c>
@@ -24842,7 +24844,7 @@
         <v>1293</v>
       </c>
     </row>
-    <row r="433" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="433" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A433" s="8" t="s">
         <v>1096</v>
       </c>
@@ -24871,7 +24873,7 @@
         <v>1096</v>
       </c>
     </row>
-    <row r="434" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="434" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A434" s="8" t="s">
         <v>1093</v>
       </c>
@@ -24900,7 +24902,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="435" spans="1:17" s="9" customFormat="1" ht="135" hidden="1" x14ac:dyDescent="0.25">
+    <row r="435" spans="1:17" s="9" customFormat="1" ht="135" x14ac:dyDescent="0.25">
       <c r="A435" s="88" t="s">
         <v>1294</v>
       </c>
@@ -24947,7 +24949,7 @@
         <v>1294</v>
       </c>
     </row>
-    <row r="436" spans="1:17" s="9" customFormat="1" ht="90" hidden="1" x14ac:dyDescent="0.25">
+    <row r="436" spans="1:17" s="9" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A436" s="19" t="s">
         <v>1296</v>
       </c>
@@ -24994,7 +24996,7 @@
         <v>1296</v>
       </c>
     </row>
-    <row r="437" spans="1:17" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="437" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A437" s="48" t="s">
         <v>1301</v>
       </c>
@@ -25038,7 +25040,7 @@
         <v>1301</v>
       </c>
     </row>
-    <row r="438" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="438" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A438" s="32" t="s">
         <v>1305</v>
       </c>
@@ -25076,7 +25078,7 @@
         <v>1305</v>
       </c>
     </row>
-    <row r="439" spans="1:17" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="439" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A439" s="28" t="s">
         <v>928</v>
       </c>
@@ -25124,7 +25126,7 @@
       </c>
       <c r="Q439" s="16"/>
     </row>
-    <row r="440" spans="1:17" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="440" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A440" s="8" t="s">
         <v>929</v>
       </c>
@@ -25172,7 +25174,7 @@
       </c>
       <c r="Q440" s="16"/>
     </row>
-    <row r="441" spans="1:17" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="441" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A441" s="3" t="s">
         <v>916</v>
       </c>
@@ -25220,7 +25222,7 @@
       </c>
       <c r="Q441" s="16"/>
     </row>
-    <row r="442" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="442" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A442" s="8" t="s">
         <v>918</v>
       </c>
@@ -25255,7 +25257,7 @@
         <v>810</v>
       </c>
     </row>
-    <row r="443" spans="1:17" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="443" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A443" s="28" t="s">
         <v>930</v>
       </c>
@@ -25303,7 +25305,7 @@
       </c>
       <c r="Q443" s="16"/>
     </row>
-    <row r="444" spans="1:17" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="444" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A444" s="8" t="s">
         <v>912</v>
       </c>
@@ -25351,7 +25353,7 @@
       </c>
       <c r="Q444" s="16"/>
     </row>
-    <row r="445" spans="1:17" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="445" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A445" s="8" t="s">
         <v>164</v>
       </c>
@@ -25401,7 +25403,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="446" spans="1:17" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="446" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A446" s="8" t="s">
         <v>919</v>
       </c>
@@ -25449,7 +25451,7 @@
       </c>
       <c r="Q446" s="16"/>
     </row>
-    <row r="447" spans="1:17" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="447" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A447" s="8" t="s">
         <v>920</v>
       </c>
@@ -25497,7 +25499,7 @@
       </c>
       <c r="Q447" s="16"/>
     </row>
-    <row r="448" spans="1:17" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="448" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A448" s="8" t="s">
         <v>921</v>
       </c>
@@ -25545,7 +25547,7 @@
       </c>
       <c r="Q448" s="16"/>
     </row>
-    <row r="449" spans="1:17" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="449" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A449" s="8" t="s">
         <v>915</v>
       </c>
@@ -25593,7 +25595,7 @@
       </c>
       <c r="Q449" s="16"/>
     </row>
-    <row r="450" spans="1:17" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="450" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A450" s="8" t="s">
         <v>913</v>
       </c>
@@ -25641,7 +25643,7 @@
       </c>
       <c r="Q450" s="16"/>
     </row>
-    <row r="451" spans="1:17" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="451" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A451" s="8" t="s">
         <v>917</v>
       </c>
@@ -25689,7 +25691,7 @@
       </c>
       <c r="Q451" s="16"/>
     </row>
-    <row r="452" spans="1:17" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="452" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A452" s="8" t="s">
         <v>165</v>
       </c>
@@ -25739,7 +25741,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="453" spans="1:17" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="453" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A453" s="8" t="s">
         <v>166</v>
       </c>
@@ -25789,7 +25791,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="454" spans="1:17" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="454" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A454" s="8" t="s">
         <v>167</v>
       </c>
@@ -25839,7 +25841,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="455" spans="1:17" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="455" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A455" s="8" t="s">
         <v>927</v>
       </c>
@@ -25884,7 +25886,7 @@
       </c>
       <c r="Q455" s="16"/>
     </row>
-    <row r="456" spans="1:17" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="456" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A456" s="3" t="s">
         <v>168</v>
       </c>
@@ -25934,7 +25936,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="457" spans="1:17" ht="345" hidden="1" x14ac:dyDescent="0.25">
+    <row r="457" spans="1:17" ht="345" x14ac:dyDescent="0.25">
       <c r="A457" s="32" t="s">
         <v>900</v>
       </c>
@@ -25982,7 +25984,7 @@
       </c>
       <c r="Q457" s="2"/>
     </row>
-    <row r="458" spans="1:17" ht="99" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="458" spans="1:17" ht="99" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A458" s="8" t="s">
         <v>1651</v>
       </c>
@@ -26023,7 +26025,7 @@
         <v>1651</v>
       </c>
     </row>
-    <row r="459" spans="1:17" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="459" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A459" s="6" t="s">
         <v>1669</v>
       </c>
@@ -26067,7 +26069,7 @@
         <v>1669</v>
       </c>
     </row>
-    <row r="460" spans="1:17" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="460" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A460" s="32" t="s">
         <v>1676</v>
       </c>
@@ -26107,7 +26109,7 @@
         <v>1677</v>
       </c>
     </row>
-    <row r="461" spans="1:17" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="461" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A461" s="19" t="s">
         <v>1678</v>
       </c>
@@ -26142,7 +26144,7 @@
         <v>1684</v>
       </c>
     </row>
-    <row r="462" spans="1:17" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="462" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A462" s="19" t="s">
         <v>1679</v>
       </c>
@@ -26177,7 +26179,7 @@
         <v>1684</v>
       </c>
     </row>
-    <row r="463" spans="1:17" s="28" customFormat="1" ht="153" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="463" spans="1:17" s="28" customFormat="1" ht="153" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A463" s="94" t="s">
         <v>1695</v>
       </c>
@@ -26224,7 +26226,7 @@
         <v>1685</v>
       </c>
     </row>
-    <row r="464" spans="1:17" ht="153" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="464" spans="1:17" ht="153" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A464" s="96" t="s">
         <v>1685</v>
       </c>
@@ -26271,7 +26273,7 @@
         <v>1685</v>
       </c>
     </row>
-    <row r="465" spans="1:15" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="465" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A465" s="49" t="s">
         <v>1689</v>
       </c>
@@ -26315,7 +26317,7 @@
         <v>1689</v>
       </c>
     </row>
-    <row r="466" spans="1:15" ht="195" hidden="1" x14ac:dyDescent="0.25">
+    <row r="466" spans="1:15" ht="195" x14ac:dyDescent="0.25">
       <c r="A466" s="32" t="s">
         <v>1700</v>
       </c>
@@ -26359,7 +26361,7 @@
         <v>1700</v>
       </c>
     </row>
-    <row r="467" spans="1:15" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="467" spans="1:15" ht="75" x14ac:dyDescent="0.25">
       <c r="A467" s="25" t="s">
         <v>1706</v>
       </c>
@@ -26403,7 +26405,7 @@
         <v>1706</v>
       </c>
     </row>
-    <row r="468" spans="1:15" s="9" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="468" spans="1:15" s="9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A468" s="22" t="s">
         <v>1711</v>
       </c>
@@ -26444,7 +26446,7 @@
         <v>1711</v>
       </c>
     </row>
-    <row r="469" spans="1:15" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="469" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D469" s="31">
         <v>43830</v>
       </c>
@@ -26456,7 +26458,7 @@
       </c>
       <c r="O469" s="11"/>
     </row>
-    <row r="470" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="470" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A470" s="22" t="s">
         <v>1715</v>
       </c>
@@ -26494,7 +26496,7 @@
         <v>1715</v>
       </c>
     </row>
-    <row r="471" spans="1:15" ht="409.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="471" spans="1:15" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A471" s="8" t="s">
         <v>1718</v>
       </c>
@@ -26532,7 +26534,7 @@
         <v>1718</v>
       </c>
     </row>
-    <row r="472" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="472" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A472" s="5" t="s">
         <v>1724</v>
       </c>
@@ -26576,7 +26578,7 @@
         <v>1724</v>
       </c>
     </row>
-    <row r="473" spans="1:15" ht="48" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="473" spans="1:15" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A473" s="97" t="s">
         <v>1729</v>
       </c>
@@ -26609,6 +26611,11 @@
       </c>
       <c r="N473" s="8" t="s">
         <v>1731</v>
+      </c>
+    </row>
+    <row r="475" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A475" s="8" t="s">
+        <v>1733</v>
       </c>
     </row>
     <row r="477" spans="1:15" x14ac:dyDescent="0.25">
@@ -26635,14 +26642,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:Q473">
-    <filterColumn colId="10">
-      <filters>
-        <filter val="TENT multipurpose, 45m², 6x7.5m + bag"/>
-        <filter val="TENT multipurpose, 72m², 12x6m + bag"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:Q473"/>
   <hyperlinks>
     <hyperlink ref="A473" r:id="rId1" tooltip="Article Fiche" display="http://portail.msfsupply.be/items/view"/>
   </hyperlinks>

</xml_diff>